<commit_message>
Update PM12 Tidsregistrering for Emil.xlsx
</commit_message>
<xml_diff>
--- a/08 Project Management/Tidsregistrering/PM12 Tidsregistrering for Emil.xlsx
+++ b/08 Project Management/Tidsregistrering/PM12 Tidsregistrering for Emil.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emiln\OneDrive\Dokumenter\HoeKulator\08 Project Management\Tidsregistrering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A83DB17D-330E-4C69-9D8C-3ADEABD89A94}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0FD55A-FC78-4BA5-BCFD-5E6DAF841FF9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Tidsregistrering af (Navn)</t>
   </si>
@@ -163,10 +163,13 @@
     <t>Review af AD1, DOM1, UC08</t>
   </si>
   <si>
-    <t>2 timer</t>
-  </si>
-  <si>
-    <t>Start på UI design prototype</t>
+    <t>Fortsættelse af UI prototype</t>
+  </si>
+  <si>
+    <t>Desktop UI design prototype</t>
+  </si>
+  <si>
+    <t>AndroidUI design prototype</t>
   </si>
 </sst>
 </file>
@@ -317,7 +320,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -358,7 +361,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -367,6 +369,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -748,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07EC185-8A27-41F3-967D-179793E73F80}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,22 +766,22 @@
     <col min="3" max="3" width="31.42578125" style="18" customWidth="1"/>
     <col min="4" max="4" width="26.7109375" style="17" customWidth="1"/>
     <col min="5" max="5" width="31" style="17" customWidth="1"/>
-    <col min="6" max="6" width="31" style="22" customWidth="1"/>
+    <col min="6" max="6" width="31" style="21" customWidth="1"/>
     <col min="7" max="7" width="37.28515625" style="6" customWidth="1"/>
     <col min="8" max="8" width="37.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -817,8 +825,8 @@
       <c r="E3" s="14">
         <v>0.54166666666666663</v>
       </c>
-      <c r="F3" s="20" t="s">
-        <v>42</v>
+      <c r="F3" s="25">
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="G3" s="5">
         <f>E3-D3</f>
@@ -831,7 +839,7 @@
     </row>
     <row r="4" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>28</v>
@@ -845,8 +853,8 @@
       <c r="E4" s="16">
         <v>0.66666666666666663</v>
       </c>
-      <c r="F4" s="21" t="s">
-        <v>42</v>
+      <c r="F4" s="24">
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="G4" s="5">
         <f t="shared" ref="G4:G32" si="0">E4-D4</f>
@@ -858,261 +866,289 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="C5" s="15"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="21"/>
+      <c r="A5" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="15">
+        <v>43886</v>
+      </c>
+      <c r="D5" s="16">
+        <v>0.4375</v>
+      </c>
+      <c r="E5" s="16">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F5" s="24">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="G5" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333315E-2</v>
       </c>
       <c r="H5" s="1">
         <f>SUM(G$3:G5)</f>
-        <v>0.24999999999999994</v>
+        <v>0.27083333333333326</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="C6" s="15"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="21"/>
+      <c r="A6" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="15">
+        <v>43886</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E6" s="16">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="F6" s="24">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="G6" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.513888888888884E-2</v>
       </c>
       <c r="H6" s="1">
         <f>SUM(G$3:G6)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C7" s="15"/>
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
-      <c r="F7" s="21"/>
+      <c r="F7" s="20"/>
       <c r="G7" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H7" s="1">
         <f>SUM(G$3:G7)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C8" s="15"/>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
-      <c r="F8" s="21"/>
+      <c r="F8" s="20"/>
       <c r="G8" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H8" s="1">
         <f>SUM(G$3:G8)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C9" s="15"/>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
-      <c r="F9" s="21"/>
+      <c r="F9" s="20"/>
       <c r="G9" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H9" s="1">
         <f>SUM(G$3:G9)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C10" s="15"/>
       <c r="D10" s="16"/>
       <c r="E10" s="16"/>
-      <c r="F10" s="21"/>
+      <c r="F10" s="20"/>
       <c r="G10" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H10" s="1">
         <f>SUM(G$3:G10)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C11" s="15"/>
       <c r="D11" s="16"/>
       <c r="E11" s="16"/>
-      <c r="F11" s="21"/>
+      <c r="F11" s="20"/>
       <c r="G11" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H11" s="1">
         <f>SUM(G$3:G11)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C12" s="15"/>
       <c r="D12" s="16"/>
       <c r="E12" s="16"/>
-      <c r="F12" s="21"/>
+      <c r="F12" s="20"/>
       <c r="G12" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H12" s="1">
         <f>SUM(G$3:G12)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C13" s="15"/>
       <c r="D13" s="16"/>
       <c r="E13" s="16"/>
-      <c r="F13" s="21"/>
+      <c r="F13" s="20"/>
       <c r="G13" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H13" s="1">
         <f>SUM(G$3:G13)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C14" s="15"/>
-      <c r="F14" s="21"/>
+      <c r="F14" s="20"/>
       <c r="G14" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H14" s="1">
         <f>SUM(G$3:G14)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C15" s="15"/>
-      <c r="F15" s="21"/>
+      <c r="F15" s="20"/>
       <c r="G15" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H15" s="1">
         <f>SUM(G$3:G15)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C16" s="15"/>
-      <c r="F16" s="21"/>
+      <c r="F16" s="20"/>
       <c r="G16" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H16" s="1">
         <f>SUM(G$3:G16)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="17" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C17" s="15"/>
-      <c r="F17" s="21"/>
+      <c r="F17" s="20"/>
       <c r="G17" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H17" s="1">
         <f>SUM(G$3:G17)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="18" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C18" s="15"/>
-      <c r="F18" s="21"/>
+      <c r="F18" s="20"/>
       <c r="G18" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H18" s="1">
         <f>SUM(G$3:G18)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="19" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C19" s="15"/>
-      <c r="F19" s="21"/>
+      <c r="F19" s="20"/>
       <c r="G19" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H19" s="1">
         <f>SUM(G$3:G19)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="20" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C20" s="15"/>
-      <c r="F20" s="21"/>
+      <c r="F20" s="20"/>
       <c r="G20" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H20" s="1">
         <f>SUM(G$3:G20)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="21" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C21" s="15"/>
-      <c r="F21" s="21"/>
+      <c r="F21" s="20"/>
       <c r="G21" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H21" s="1">
         <f>SUM(G$3:G21)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="22" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C22" s="15"/>
-      <c r="F22" s="21"/>
+      <c r="F22" s="20"/>
       <c r="G22" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H22" s="1">
         <f>SUM(G$3:G22)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="23" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C23" s="15"/>
-      <c r="F23" s="21"/>
+      <c r="F23" s="20"/>
       <c r="G23" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H23" s="1">
         <f>SUM(G$3:G23)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="24" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
       <c r="C24" s="15"/>
-      <c r="F24" s="21"/>
+      <c r="F24" s="20"/>
       <c r="G24" s="5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H24" s="1">
         <f>SUM(G$3:G24)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="25" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1123,7 +1159,7 @@
       </c>
       <c r="H25" s="1">
         <f>SUM(G$3:G25)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="26" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1134,7 +1170,7 @@
       </c>
       <c r="H26" s="1">
         <f>SUM(G$3:G26)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="27" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1145,7 +1181,7 @@
       </c>
       <c r="H27" s="1">
         <f>SUM(G$3:G27)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="28" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1156,7 +1192,7 @@
       </c>
       <c r="H28" s="1">
         <f>SUM(G$3:G28)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="29" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1167,7 +1203,7 @@
       </c>
       <c r="H29" s="1">
         <f>SUM(G$3:G29)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="30" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1178,7 +1214,7 @@
       </c>
       <c r="H30" s="1">
         <f>SUM(G$3:G30)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="31" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1189,7 +1225,7 @@
       </c>
       <c r="H31" s="1">
         <f>SUM(G$3:G31)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="32" spans="3:8" ht="19.5" x14ac:dyDescent="0.3">
@@ -1200,7 +1236,7 @@
       </c>
       <c r="H32" s="1">
         <f>SUM(G$3:G32)</f>
-        <v>0.24999999999999994</v>
+        <v>0.3159722222222221</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.25">
@@ -1285,13 +1321,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">

</xml_diff>